<commit_message>
First table with AIC/BIC/logL values
</commit_message>
<xml_diff>
--- a/RaxML_analysis/RAxML_run_summary.xlsx
+++ b/RaxML_analysis/RAxML_run_summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pollo\Documents\Box Sync\EEOB563\EEOB563_S19FinalProject\seq\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pollo\Documents\Box Sync\EEOB563\EEOB563_S19FinalProject\RaxML_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6CC113-6429-4C4C-AC0C-92818FF6E220}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01307FAA-47D2-4555-AFE5-E1CC1F79AB28}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3A8E787D-85F8-4AF4-B4A9-9C09B004D04D}"/>
+    <workbookView xWindow="3225" yWindow="1305" windowWidth="21975" windowHeight="11490" xr2:uid="{3A8E787D-85F8-4AF4-B4A9-9C09B004D04D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="55">
   <si>
     <t>RunName</t>
   </si>
@@ -187,6 +187,15 @@
   </si>
   <si>
     <t>RaxML_____________21</t>
+  </si>
+  <si>
+    <t>AIC</t>
+  </si>
+  <si>
+    <t>BIC</t>
+  </si>
+  <si>
+    <t>Final LogLikelihood</t>
   </si>
 </sst>
 </file>
@@ -546,23 +555,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5F246AD-F8A7-4AB0-8D93-D301BD698F09}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -581,19 +592,28 @@
       <c r="F1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1">
-        <v>-13153.313185999999</v>
+        <v>-13017.26355</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>16</v>
@@ -601,19 +621,28 @@
       <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="1">
+        <v>27166.084647</v>
+      </c>
+      <c r="H2" s="1">
+        <v>27971.412735999998</v>
+      </c>
+      <c r="I2" s="1">
+        <v>-13397.042324</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1">
-        <v>-13017.26355</v>
+        <v>-13153.313185999999</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>16</v>
@@ -621,19 +650,28 @@
       <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="1">
+        <v>27251.656081000001</v>
+      </c>
+      <c r="H3" s="1">
+        <v>28056.98417</v>
+      </c>
+      <c r="I3" s="1">
+        <v>-13439.828041000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1">
-        <v>-4911.59584</v>
+        <v>-4809.521189</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>16</v>
@@ -641,19 +679,28 @@
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="1">
+        <v>10670.111351</v>
+      </c>
+      <c r="H4" s="1">
+        <v>11531.184984</v>
+      </c>
+      <c r="I4" s="1">
+        <v>-5119.0556759999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1">
-        <v>-4809.521189</v>
+        <v>-4911.59584</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
@@ -661,19 +708,28 @@
       <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="1">
+        <v>10861.476567</v>
+      </c>
+      <c r="H5" s="1">
+        <v>11722.5502</v>
+      </c>
+      <c r="I5" s="1">
+        <v>-5214.7382829999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1">
-        <v>-5415.7299329999996</v>
+        <v>-5363.3064430000004</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
@@ -681,19 +737,28 @@
       <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="1">
+        <v>10967.754516000001</v>
+      </c>
+      <c r="H6" s="1">
+        <v>11191.833748999999</v>
+      </c>
+      <c r="I6" s="1">
+        <v>-5427.8772580000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1">
-        <v>-5363.3064430000004</v>
+        <v>-5415.7299329999996</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
@@ -701,8 +766,17 @@
       <c r="F7" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="1">
+        <v>11030.858383000001</v>
+      </c>
+      <c r="H7" s="1">
+        <v>11254.937615999999</v>
+      </c>
+      <c r="I7" s="1">
+        <v>-5459.4291910000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
@@ -721,8 +795,17 @@
       <c r="F8" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="1">
+        <v>59826.810312000001</v>
+      </c>
+      <c r="H8" s="1">
+        <v>61123.825406999997</v>
+      </c>
+      <c r="I8" s="1">
+        <v>-29697.405156000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -741,36 +824,54 @@
       <c r="F9" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="G9" s="1">
+        <v>59837.818930000001</v>
+      </c>
+      <c r="H9" s="1">
+        <v>61134.834024999996</v>
+      </c>
+      <c r="I9" s="1">
+        <v>-29702.909465000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1">
+        <v>-99416.866563000003</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="1">
+        <v>209942.24200200001</v>
+      </c>
+      <c r="H10" s="1">
+        <v>211569.32715500001</v>
+      </c>
+      <c r="I10" s="1">
+        <v>-104723.12100100001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="1">
-        <v>-99416.866563000003</v>
+        <v>12</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>16</v>
@@ -778,8 +879,17 @@
       <c r="F11" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="1">
+        <v>210121.32786799999</v>
+      </c>
+      <c r="H11" s="1">
+        <v>211748.41302099999</v>
+      </c>
+      <c r="I11" s="1">
+        <v>-104812.663934</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -798,19 +908,28 @@
       <c r="F12" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="1">
+        <v>190411.97349800001</v>
+      </c>
+      <c r="H12" s="1">
+        <v>191988.930131</v>
+      </c>
+      <c r="I12" s="1">
+        <v>-94967.986749000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" s="1">
-        <v>-29567.364072</v>
+        <v>-28995.531053999999</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>16</v>
@@ -818,19 +937,28 @@
       <c r="F13" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="1">
+        <v>60950.063335999999</v>
+      </c>
+      <c r="H13" s="1">
+        <v>62107.433187000002</v>
+      </c>
+      <c r="I13" s="1">
+        <v>-30259.031668</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="1">
-        <v>-28995.531053999999</v>
+        <v>-29567.364072</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>16</v>
@@ -838,8 +966,17 @@
       <c r="F14" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="1">
+        <v>62088.057613999998</v>
+      </c>
+      <c r="H14" s="1">
+        <v>63245.427464</v>
+      </c>
+      <c r="I14" s="1">
+        <v>-30828.028806999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -859,7 +996,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -879,7 +1016,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
@@ -899,136 +1036,189 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="1">
+        <v>-31479.332747</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="1">
+        <v>64698.132706999997</v>
+      </c>
+      <c r="H18" s="1">
+        <v>65027.930120999998</v>
+      </c>
+      <c r="I18" s="1">
+        <v>-32291.066353999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D19" s="1">
         <v>-31810.059519999999</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="2">
-        <v>-31479.332747</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="E19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="1">
+        <v>64928.663383999999</v>
+      </c>
+      <c r="H19" s="1">
+        <v>65258.460797</v>
+      </c>
+      <c r="I19" s="1">
+        <v>-32406.331692</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1">
+        <v>-70926.891969000004</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="1">
+        <v>149741.45392999999</v>
+      </c>
+      <c r="H20" s="1">
+        <v>150994.64281700001</v>
+      </c>
+      <c r="I20" s="1">
+        <v>-74654.726964999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D21" s="1">
         <v>-72124.902675000005</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="2">
-        <v>-70926.891969000004</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="E21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="1">
+        <v>151631.367341</v>
+      </c>
+      <c r="H21" s="1">
+        <v>152884.55622699999</v>
+      </c>
+      <c r="I21" s="1">
+        <v>-75599.683669999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="1">
+        <v>-116832.449767</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="1">
+        <v>428254.29828300001</v>
+      </c>
+      <c r="H22" s="1">
+        <v>429832.08793500002</v>
+      </c>
+      <c r="I22" s="1">
+        <v>-213915.14914200001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="2">
-        <v>-116832.449767</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="1">
+        <v>429043.882293</v>
+      </c>
+      <c r="H23" s="1">
+        <v>430621.67194500001</v>
+      </c>
+      <c r="I23" s="1">
+        <v>-214309.941146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D24" s="1">
-        <v>-38203.595950000003</v>
+        <v>-37352.607713999998</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>16</v>
@@ -1036,19 +1226,28 @@
       <c r="F24" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G24" s="1">
+        <v>79872.396766999998</v>
+      </c>
+      <c r="H24" s="1">
+        <v>81136.187422999996</v>
+      </c>
+      <c r="I24" s="1">
+        <v>-39720.198383000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D25" s="1">
-        <v>-37352.607713999998</v>
+        <v>-38203.595950000003</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>16</v>
@@ -1056,19 +1255,28 @@
       <c r="F25" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="1">
+        <v>81527.181821000006</v>
+      </c>
+      <c r="H25" s="1">
+        <v>82790.972475999995</v>
+      </c>
+      <c r="I25" s="1">
+        <v>-40547.590909999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D26" s="1">
-        <v>-45328.390428999999</v>
+        <v>-44673.667219000003</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>16</v>
@@ -1076,19 +1284,28 @@
       <c r="F26" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G26" s="1">
+        <v>92140.823103999996</v>
+      </c>
+      <c r="H26" s="1">
+        <v>92465.739902000001</v>
+      </c>
+      <c r="I26" s="1">
+        <v>-46016.411551999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D27" s="1">
-        <v>-44673.667219000003</v>
+        <v>-45328.390428999999</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>16</v>
@@ -1096,49 +1313,75 @@
       <c r="F27" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G27" s="1">
+        <v>92868.515927999993</v>
+      </c>
+      <c r="H27" s="1">
+        <v>93193.432725999999</v>
+      </c>
+      <c r="I27" s="1">
+        <v>-46380.257963999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="1">
+        <v>243770.05381000001</v>
+      </c>
+      <c r="H28" s="1">
+        <v>245221.14382500001</v>
+      </c>
+      <c r="I28" s="1">
+        <v>-121669.02690500001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D29" s="1">
         <v>-118676.162627</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>15</v>
+      <c r="E29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="1">
+        <v>246661.68105399999</v>
+      </c>
+      <c r="H29" s="1">
+        <v>248112.77106999999</v>
+      </c>
+      <c r="I29" s="1">
+        <v>-123114.84052699999</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F29">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I29">
     <sortCondition ref="B2:B29"/>
-    <sortCondition ref="C2:C29"/>
+    <sortCondition ref="G2:G29"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixing errors in phytozome datasets
</commit_message>
<xml_diff>
--- a/RaxML_analysis/RAxML_run_summary.xlsx
+++ b/RaxML_analysis/RAxML_run_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pollo\Documents\Box Sync\EEOB563\EEOB563_S19FinalProject\RaxML_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01307FAA-47D2-4555-AFE5-E1CC1F79AB28}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785107AD-F66C-49E5-AC00-670B90C2C360}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3225" yWindow="1305" windowWidth="21975" windowHeight="11490" xr2:uid="{3A8E787D-85F8-4AF4-B4A9-9C09B004D04D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3A8E787D-85F8-4AF4-B4A9-9C09B004D04D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="55">
   <si>
     <t>RunName</t>
   </si>
@@ -162,9 +162,6 @@
     <t>RaxML__________21</t>
   </si>
   <si>
-    <t>RaxML___________22</t>
-  </si>
-  <si>
     <t>RaxML__14</t>
   </si>
   <si>
@@ -180,9 +177,6 @@
     <t>RaxML_____________23</t>
   </si>
   <si>
-    <t>RaxML______________23</t>
-  </si>
-  <si>
     <t>RaxML____________20</t>
   </si>
   <si>
@@ -196,6 +190,12 @@
   </si>
   <si>
     <t>Final LogLikelihood</t>
+  </si>
+  <si>
+    <t>RaxML_TOR_LG</t>
+  </si>
+  <si>
+    <t>RaxML_TOR_B62</t>
   </si>
 </sst>
 </file>
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5F246AD-F8A7-4AB0-8D93-D301BD698F09}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -593,13 +593,13 @@
         <v>30</v>
       </c>
       <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" t="s">
         <v>52</v>
-      </c>
-      <c r="H1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -776,61 +776,61 @@
         <v>-5459.4291910000002</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>-29500.945144000001</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="1">
+      <c r="E8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="2">
         <v>59826.810312000001</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="2">
         <v>61123.825406999997</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="2">
         <v>-29697.405156000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="1">
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2">
         <v>-29368.363826000001</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="1">
+      <c r="E9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="2">
         <v>59837.818930000001</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="2">
         <v>61134.834024999996</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="2">
         <v>-29702.909465000001</v>
       </c>
     </row>
@@ -865,7 +865,7 @@
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>18</v>
@@ -1038,7 +1038,7 @@
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>32</v>
@@ -1067,7 +1067,7 @@
     </row>
     <row r="19" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>32</v>
@@ -1094,67 +1094,67 @@
         <v>-32406.331692</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="2">
+        <v>-70926.891969000004</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="2">
+        <v>149741.45392999999</v>
+      </c>
+      <c r="H20" s="2">
+        <v>150994.64281700001</v>
+      </c>
+      <c r="I20" s="2">
+        <v>-74654.726964999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="1">
-        <v>-70926.891969000004</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="1">
-        <v>149741.45392999999</v>
-      </c>
-      <c r="H20" s="1">
-        <v>150994.64281700001</v>
-      </c>
-      <c r="I20" s="1">
-        <v>-74654.726964999994</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="2">
         <v>-72124.902675000005</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="1">
+      <c r="E21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="2">
         <v>151631.367341</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="2">
         <v>152884.55622699999</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I21" s="2">
         <v>-75599.683669999999</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>25</v>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="23" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>25</v>
@@ -1323,58 +1323,58 @@
         <v>-46380.257963999997</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="1" t="s">
+    <row r="28" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" s="1">
+      <c r="C28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="2">
         <v>243770.05381000001</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28" s="2">
         <v>245221.14382500001</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I28" s="2">
         <v>-121669.02690500001</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="1" t="s">
+    <row r="29" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="2">
         <v>-118676.162627</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G29" s="1">
+      <c r="E29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="2">
         <v>246661.68105399999</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="2">
         <v>248112.77106999999</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I29" s="2">
         <v>-123114.84052699999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished intro / archived old analysis files
</commit_message>
<xml_diff>
--- a/RaxML_analysis/RAxML_run_summary.xlsx
+++ b/RaxML_analysis/RAxML_run_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pollo\Documents\Box Sync\EEOB563\EEOB563_S19FinalProject\RaxML_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785107AD-F66C-49E5-AC00-670B90C2C360}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BABD9F-5D91-4D54-B3A7-9EA17F042207}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3A8E787D-85F8-4AF4-B4A9-9C09B004D04D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="55">
   <si>
     <t>RunName</t>
   </si>
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5F246AD-F8A7-4AB0-8D93-D301BD698F09}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -776,62 +776,62 @@
         <v>-5459.4291910000002</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-29368.363826000001</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="1">
+        <v>59912.367238999999</v>
+      </c>
+      <c r="H8" s="1">
+        <v>61220.954566</v>
+      </c>
+      <c r="I8" s="1">
+        <v>-29738.183618999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D9" s="1">
         <v>-29500.945144000001</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="2">
-        <v>59826.810312000001</v>
-      </c>
-      <c r="H8" s="2">
-        <v>61123.825406999997</v>
-      </c>
-      <c r="I8" s="2">
-        <v>-29697.405156000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2">
-        <v>-29368.363826000001</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="2">
-        <v>59837.818930000001</v>
-      </c>
-      <c r="H9" s="2">
-        <v>61134.834024999996</v>
-      </c>
-      <c r="I9" s="2">
-        <v>-29702.909465000001</v>
+      <c r="E9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="1">
+        <v>59933.435596000003</v>
+      </c>
+      <c r="H9" s="1">
+        <v>61242.022922999997</v>
+      </c>
+      <c r="I9" s="1">
+        <v>-29748.717798000001</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1094,62 +1094,62 @@
         <v>-32406.331692</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="2">
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1">
         <v>-70926.891969000004</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="2">
-        <v>149741.45392999999</v>
-      </c>
-      <c r="H20" s="2">
-        <v>150994.64281700001</v>
-      </c>
-      <c r="I20" s="2">
-        <v>-74654.726964999994</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+      <c r="E20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="1">
+        <v>149858.93192100001</v>
+      </c>
+      <c r="H20" s="1">
+        <v>151123.81355200001</v>
+      </c>
+      <c r="I20" s="1">
+        <v>-74711.465960000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>-72124.902675000005</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="2">
-        <v>151631.367341</v>
-      </c>
-      <c r="H21" s="2">
-        <v>152884.55622699999</v>
-      </c>
-      <c r="I21" s="2">
-        <v>-75599.683669999999</v>
+      <c r="E21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="1">
+        <v>151740.83620300001</v>
+      </c>
+      <c r="H21" s="1">
+        <v>153005.71783400001</v>
+      </c>
+      <c r="I21" s="1">
+        <v>-75652.418101000003</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1323,59 +1323,59 @@
         <v>-46380.257963999997</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" s="2">
-        <v>243770.05381000001</v>
-      </c>
-      <c r="H28" s="2">
-        <v>245221.14382500001</v>
-      </c>
-      <c r="I28" s="2">
-        <v>-121669.02690500001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
+      <c r="C28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="1">
+        <v>243948.52570900001</v>
+      </c>
+      <c r="H28" s="1">
+        <v>245413.69281499999</v>
+      </c>
+      <c r="I28" s="1">
+        <v>-121756.262854</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="1">
         <v>-118676.162627</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G29" s="2">
-        <v>246661.68105399999</v>
-      </c>
-      <c r="H29" s="2">
-        <v>248112.77106999999</v>
-      </c>
-      <c r="I29" s="2">
-        <v>-123114.84052699999</v>
+      <c r="E29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="1">
+        <v>246850.437068</v>
+      </c>
+      <c r="H29" s="1">
+        <v>248315.60417400001</v>
+      </c>
+      <c r="I29" s="1">
+        <v>-123207.218534</v>
       </c>
     </row>
   </sheetData>

</xml_diff>